<commit_message>
refactor to fit package installation
</commit_message>
<xml_diff>
--- a/data/students_with_groups.xlsx
+++ b/data/students_with_groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcdermott/code/github/appt-scheduling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8B0E9F-4F26-1D46-81EB-6BEBF924BEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A42BF0-7588-1D40-BBBD-11AA664B4030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="760" windowWidth="22580" windowHeight="17440" xr2:uid="{A4A0CDEB-AD60-4A4B-A382-7E2316AE69E9}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="22580" windowHeight="17440" xr2:uid="{A4A0CDEB-AD60-4A4B-A382-7E2316AE69E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -218,33 +218,9 @@
     <t>Stuppi_2</t>
   </si>
   <si>
-    <t>T_K RTI_1</t>
-  </si>
-  <si>
-    <t>T_K RTI_2</t>
-  </si>
-  <si>
-    <t>B_E_1</t>
-  </si>
-  <si>
-    <t>B_E_2</t>
-  </si>
-  <si>
-    <t>A_I_1</t>
-  </si>
-  <si>
-    <t>s_z_1</t>
-  </si>
-  <si>
-    <t>s_z_2</t>
-  </si>
-  <si>
     <t>5th_2</t>
   </si>
   <si>
-    <t>ASSESSMENT</t>
-  </si>
-  <si>
     <t>LUNCH_1</t>
   </si>
   <si>
@@ -252,6 +228,33 @@
   </si>
   <si>
     <t>LUNCH_3</t>
+  </si>
+  <si>
+    <t>ASSESSMENT_1</t>
+  </si>
+  <si>
+    <t>ASSESSMENT_2</t>
+  </si>
+  <si>
+    <t>T+K+RTI_1</t>
+  </si>
+  <si>
+    <t>T+K+RTI_2</t>
+  </si>
+  <si>
+    <t>B+E_1</t>
+  </si>
+  <si>
+    <t>B+E_2</t>
+  </si>
+  <si>
+    <t>A+I_1</t>
+  </si>
+  <si>
+    <t>s+z_1</t>
+  </si>
+  <si>
+    <t>s+z_2</t>
   </si>
 </sst>
 </file>
@@ -642,12 +645,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2912BC91-4312-014C-AB0B-89A6258E9047}">
-  <dimension ref="A1:AK36"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="134" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A30" sqref="A30"/>
-      <selection pane="topRight" activeCell="G36" sqref="G36"/>
+      <selection pane="topRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,7 +798,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -872,7 +875,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1343,7 +1346,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1411,7 +1414,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1583,7 +1586,7 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1715,7 +1718,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1783,7 +1786,7 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2839,7 +2842,7 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -2892,7 +2895,7 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C32">
         <v>15</v>
@@ -2912,13 +2915,13 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C33">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2953,10 +2956,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C34">
         <v>30</v>
@@ -2968,55 +2971,96 @@
         <v>1</v>
       </c>
       <c r="F34" s="5">
-        <v>0.46875</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="G34" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="H34" s="3">
+        <v>2</v>
+      </c>
+      <c r="I34" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="J34" s="5">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="K34" s="3">
+        <v>5</v>
+      </c>
+      <c r="L34" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="M34" s="5">
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C35">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" s="5">
-        <v>0.46875</v>
+        <v>0.46527777777777773</v>
       </c>
       <c r="G35" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.52430555555555558</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C36">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F36" s="5">
-        <v>0.46875</v>
+        <v>0.46527777777777773</v>
       </c>
       <c r="G36" s="5">
+        <v>0.52430555555555558</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37">
+        <v>-1</v>
+      </c>
+      <c r="C37">
+        <v>25</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3">
+        <v>5</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="G37" s="5">
         <v>0.50694444444444442</v>
       </c>
     </row>

</xml_diff>